<commit_message>
los and nlos done
</commit_message>
<xml_diff>
--- a/Tests/test results.xlsx
+++ b/Tests/test results.xlsx
@@ -435,7 +435,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,6 +508,9 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -545,6 +548,9 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -581,6 +587,9 @@
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>11</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>